<commit_message>
Initial commit: add main.py, queries.sql, README.md, requirements.txt
</commit_message>
<xml_diff>
--- a/query_results.xlsx
+++ b/query_results.xlsx
@@ -11,13 +11,19 @@
     <sheet name="Customers unique id with order " sheetId="2" r:id="rId2"/>
     <sheet name="Average product price" sheetId="3" r:id="rId3"/>
     <sheet name="Top 5 categories of products" sheetId="4" r:id="rId4"/>
+    <sheet name="average time of delivery" sheetId="5" r:id="rId5"/>
+    <sheet name="average order check" sheetId="6" r:id="rId6"/>
+    <sheet name="top five cities by amount of cu" sheetId="7" r:id="rId7"/>
+    <sheet name="How many reviews with every sco" sheetId="8" r:id="rId8"/>
+    <sheet name="Tob 5 sellers by revenue" sheetId="9" r:id="rId9"/>
+    <sheet name="Number of orders by years" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>count</t>
   </si>
@@ -122,6 +128,87 @@
   </si>
   <si>
     <t>informatica_acessorios</t>
+  </si>
+  <si>
+    <t>avg_delay_days</t>
+  </si>
+  <si>
+    <t>-11.88</t>
+  </si>
+  <si>
+    <t>avg_order_value</t>
+  </si>
+  <si>
+    <t>137.75</t>
+  </si>
+  <si>
+    <t>customer_city</t>
+  </si>
+  <si>
+    <t>total_customers</t>
+  </si>
+  <si>
+    <t>sao paulo</t>
+  </si>
+  <si>
+    <t>rio de janeiro</t>
+  </si>
+  <si>
+    <t>belo horizonte</t>
+  </si>
+  <si>
+    <t>brasilia</t>
+  </si>
+  <si>
+    <t>curitiba</t>
+  </si>
+  <si>
+    <t>review_score</t>
+  </si>
+  <si>
+    <t>count_reviews</t>
+  </si>
+  <si>
+    <t>seller_id</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>4869f7a5dfa277a7dca6462dcf3b52b2</t>
+  </si>
+  <si>
+    <t>53243585a1d6dc2643021fd1853d8905</t>
+  </si>
+  <si>
+    <t>4a3ca9315b744ce9f8e9374361493884</t>
+  </si>
+  <si>
+    <t>fa1c13f2614d7b5c4749cbc52fecda94</t>
+  </si>
+  <si>
+    <t>7c67e1448b00f6e969d365cea6b010ab</t>
+  </si>
+  <si>
+    <t>229472.63</t>
+  </si>
+  <si>
+    <t>222776.05</t>
+  </si>
+  <si>
+    <t>200472.92</t>
+  </si>
+  <si>
+    <t>194042.03</t>
+  </si>
+  <si>
+    <t>187923.89</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>total_orders</t>
   </si>
 </sst>
 </file>
@@ -500,6 +587,51 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2016</v>
+      </c>
+      <c r="B2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2017</v>
+      </c>
+      <c r="B3">
+        <v>45101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2018</v>
+      </c>
+      <c r="B4">
+        <v>54011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
@@ -716,4 +848,233 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>15540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>6882</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>1521</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>11424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>19142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>57328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>